<commit_message>
Seccion de contacto y copia de plantillas
</commit_message>
<xml_diff>
--- a/productos/categorias.xlsx
+++ b/productos/categorias.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Adrián\Documentos\Argentina programa 4.0\PaginaGalpon\productos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PaginaGalpon\productos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="350">
   <si>
     <t>Rayadas</t>
   </si>
@@ -739,24 +739,12 @@
     <t>/img/pizzera-en-chapa-enlozada.jpg</t>
   </si>
   <si>
-    <t>Cacerolas de fundicion Ovaladas</t>
-  </si>
-  <si>
-    <t>Cacerolas de fundicion doble función</t>
-  </si>
-  <si>
     <t>Planchas para bifes lisas</t>
   </si>
   <si>
     <t>Planchas para bifes rayadas</t>
   </si>
   <si>
-    <t>Provoleteras de fundición mangos de madera</t>
-  </si>
-  <si>
-    <t>Provoleteras de fundición mangos de fundición</t>
-  </si>
-  <si>
     <t>Provoleteras de 15 porciones</t>
   </si>
   <si>
@@ -841,12 +829,6 @@
     <t>/productos/Categorias/Gastronomia/Planchas-para-bifes/Planchas-para-bifes-rayadas.html</t>
   </si>
   <si>
-    <t>/productos/Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mangos-de-madera.html</t>
-  </si>
-  <si>
-    <t>/productos/Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mangos-de-fundicion.html</t>
-  </si>
-  <si>
     <t>Muebles de jardin en Fundición de aluminio</t>
   </si>
   <si>
@@ -928,12 +910,6 @@
     <t>/img/provoleteras-de-fundicion.jpg</t>
   </si>
   <si>
-    <t>/img/provoleteras-de-fundicion-mangos-de-madera.jpg</t>
-  </si>
-  <si>
-    <t>/img/provoleteras-de-fundicion-mangos-de-fundicion.jpg</t>
-  </si>
-  <si>
     <t>/img/provoleteras-de-15-porciones.jpg</t>
   </si>
   <si>
@@ -964,12 +940,6 @@
     <t>/img/cacerolas-de-fundicion-sin-enlozar.jpg</t>
   </si>
   <si>
-    <t>/productos/Categorias/Gastronomia/Cacerolas-de-fundicion/Cacerolas-de-fundicion-sin-enlozar/Cacerolas-de-fundicion-Ovaladas.html</t>
-  </si>
-  <si>
-    <t>/productos/Categorias/Gastronomia/Cacerolas-de-fundicion/Cacerolas-de-fundicion-sin-enlozar/Cacerolas-de-fundicion-doble-funcion.html</t>
-  </si>
-  <si>
     <t>Planchas para bifes rayadas enlozadas</t>
   </si>
   <si>
@@ -982,36 +952,6 @@
     <t>/productos/Categorias/Gastronomia/Planchas-para-bifes/Planchas-para-bifes-rayadas/Planchas-para-bifes-rayadas-sin-enlozar.html</t>
   </si>
   <si>
-    <t>Provoleteras de fundición mangos de madera enlozadas</t>
-  </si>
-  <si>
-    <t>/productos/Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mangos-de-madera/Provoleteras-de-fundicion-mangos-de-madera-enlozadas.html</t>
-  </si>
-  <si>
-    <t>/img/provoleteras-de-fundicion-mangos-de-madera-enlozadas.jpg</t>
-  </si>
-  <si>
-    <t>Provoleteras de fundición mangos de madera sin enlozar</t>
-  </si>
-  <si>
-    <t>/productos/Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mangos-de-madera/Provoleteras-de-fundicion-mangos-de-madera-sin-enlozar.html</t>
-  </si>
-  <si>
-    <t>/img/provoleteras-de-fundicion-mangos-de-madera-sin-enlozar.jpg</t>
-  </si>
-  <si>
-    <t>/productos/Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mangos-de-fundicion/Provoleteras-de-fundicion-mangos-de-fundicion-enlozadas.html</t>
-  </si>
-  <si>
-    <t>/img/provoleteras-de-fundicion-mangos-de-enlozadas.jpg</t>
-  </si>
-  <si>
-    <t>/productos/Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mangos-de-fundicion/Provoleteras-de-fundicion-mangos-de-fundicion-sin-enlozar.html</t>
-  </si>
-  <si>
-    <t>/img/provoleteras-de-fundicion-mangos-de-sin-enlozar.jpg</t>
-  </si>
-  <si>
     <t>Provoleteras de 15 porciones enlozadas</t>
   </si>
   <si>
@@ -1069,21 +1009,92 @@
     <t>/productos/Categorias/Gastronomia/Sarten-mango-de-planchuela.html</t>
   </si>
   <si>
-    <t>Provoleteras de fundicion mangos de fundicion enlozadas</t>
-  </si>
-  <si>
-    <t>Provoleteras de fundicion mangos de enlozadas</t>
-  </si>
-  <si>
-    <t>Provoleteras de fundicion mangos de fundicion sin enlozar</t>
+    <t>/productos/Categorias/Gastronomia/Cacerolas-de-fundicion/Cacerolas-de-fundicion-sin-enlozar/Cacerolas-de-fundicion-sin-enlozar-ovaladas.html</t>
+  </si>
+  <si>
+    <t>/productos/Categorias/Gastronomia/Cacerolas-de-fundicion/Cacerolas-de-fundicion-sin-enlozar/Cacerolas-de-fundicion-sin-enlozar-doble-funcion.html</t>
+  </si>
+  <si>
+    <t>/productos/Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-madera.html</t>
+  </si>
+  <si>
+    <t>/productos/Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-madera/Provoleteras-de-fundicion-mango-de-madera-enlozadas.html</t>
+  </si>
+  <si>
+    <t>/productos/Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-madera/Provoleteras-de-fundicion-mango-de-madera-sin-enlozar.html</t>
+  </si>
+  <si>
+    <t>/productos/Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion.html</t>
+  </si>
+  <si>
+    <t>Provoleteras de fundición mango de madera</t>
+  </si>
+  <si>
+    <t>/img/provoleteras-de-fundicion-mango-de-madera.jpg</t>
+  </si>
+  <si>
+    <t>Provoleteras de fundición mango de madera enlozadas</t>
+  </si>
+  <si>
+    <t>/img/provoleteras-de-fundicion-mango-de-madera-enlozadas.jpg</t>
+  </si>
+  <si>
+    <t>Provoleteras de fundición mango de madera sin enlozar</t>
+  </si>
+  <si>
+    <t>/img/provoleteras-de-fundicion-mango-de-madera-sin-enlozar.jpg</t>
+  </si>
+  <si>
+    <t>Provoleteras de fundición mango de fundición</t>
+  </si>
+  <si>
+    <t>/img/provoleteras-de-fundicion-mango-de-fundicion.jpg</t>
+  </si>
+  <si>
+    <t>Provoleteras de fundicion mango de fundicion enlozadas</t>
+  </si>
+  <si>
+    <t>/productos/Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion-enlozadas.html</t>
+  </si>
+  <si>
+    <t>/img/provoleteras-de-fundicion-mango-de-enlozadas.jpg</t>
+  </si>
+  <si>
+    <t>Provoleteras de fundicion mango de fundicion sin enlozar</t>
+  </si>
+  <si>
+    <t>/productos/Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion-sin-enlozar.html</t>
+  </si>
+  <si>
+    <t>/img/provoleteras-de-fundicion-mango-de-sin-enlozar.jpg</t>
+  </si>
+  <si>
+    <t>Cacerolas de fundicion sin enlozar ovaladas</t>
+  </si>
+  <si>
+    <t>Cacerolas de fundicion sin enlozar doble función</t>
+  </si>
+  <si>
+    <t>Para usar el MD para crear la ruta de carpetas</t>
+  </si>
+  <si>
+    <t>Para usar el COPY para copiar la plantilla a todas las carpetas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1195,7 +1206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1211,6 +1222,22 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1491,33 +1518,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39:B40"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2:L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="126" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="53.28515625" customWidth="1"/>
+    <col min="3" max="3" width="169.7109375" customWidth="1"/>
     <col min="4" max="4" width="55.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.5703125" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" customWidth="1"/>
-    <col min="8" max="8" width="44.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="30" customWidth="1"/>
+    <col min="9" max="10" width="1.140625" customWidth="1"/>
+    <col min="11" max="11" width="147.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="152.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="15" t="s">
         <v>50</v>
       </c>
       <c r="D1" t="s">
@@ -1532,20 +1562,22 @@
       <c r="G1" t="s">
         <v>53</v>
       </c>
-      <c r="H1" t="str">
-        <f>CONCATENATE("copy H8")</f>
-        <v>copy H8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>348</v>
+      </c>
+      <c r="L1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>252</v>
+      <c r="C2" s="16" t="s">
+        <v>248</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>150</v>
@@ -1556,19 +1588,36 @@
       <c r="G2" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="30"/>
+      <c r="I2" s="6" t="str">
+        <f>SUBSTITUTE(C2,"/productos/","")</f>
+        <v>Categorias/Jardin.html</v>
+      </c>
+      <c r="J2" s="6" t="str">
+        <f t="shared" ref="J2:J33" si="0">SUBSTITUTE(I2,".html","")</f>
+        <v>Categorias/Jardin</v>
+      </c>
+      <c r="K2" s="6" t="str">
+        <f>SUBSTITUTE(J2,"/","\")</f>
+        <v>Categorias\Jardin</v>
+      </c>
+      <c r="L2" s="6" t="str">
+        <f>CONCATENATE("copy plantilla-categorias.html ",(SUBSTITUTE(I2,"/","\")))</f>
+        <v>copy plantilla-categorias.html Categorias\Jardin.html</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>243</v>
+      <c r="C3" s="17" t="s">
+        <v>239</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="E3" s="7">
         <v>1</v>
@@ -1579,16 +1628,33 @@
       <c r="G3" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="30"/>
+      <c r="I3" s="7" t="str">
+        <f t="shared" ref="I3:I52" si="1">SUBSTITUTE(C3,"/productos/","")</f>
+        <v>Categorias/Jardin/Arrollamangueras.html</v>
+      </c>
+      <c r="J3" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Jardin/Arrollamangueras</v>
+      </c>
+      <c r="K3" s="7" t="str">
+        <f t="shared" ref="K3:K52" si="2">SUBSTITUTE(J3,"/","\")</f>
+        <v>Categorias\Jardin\Arrollamangueras</v>
+      </c>
+      <c r="L3" s="7" t="str">
+        <f t="shared" ref="L3:L52" si="3">CONCATENATE("copy plantilla-categorias.html ",(SUBSTITUTE(I3,"/","\")))</f>
+        <v>copy plantilla-categorias.html Categorias\Jardin\Arrollamangueras.html</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>244</v>
+      <c r="C4" s="17" t="s">
+        <v>240</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>155</v>
@@ -1602,19 +1668,36 @@
       <c r="G4" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="30"/>
+      <c r="I4" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Jardin/Bebederos.html</v>
+      </c>
+      <c r="J4" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Jardin/Bebederos</v>
+      </c>
+      <c r="K4" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Jardin\Bebederos</v>
+      </c>
+      <c r="L4" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Jardin\Bebederos.html</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>245</v>
+      <c r="C5" s="17" t="s">
+        <v>241</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="E5" s="7">
         <v>1</v>
@@ -1625,19 +1708,36 @@
       <c r="G5" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="30"/>
+      <c r="I5" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Jardin/Llamadores.html</v>
+      </c>
+      <c r="J5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Jardin/Llamadores</v>
+      </c>
+      <c r="K5" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Jardin\Llamadores</v>
+      </c>
+      <c r="L5" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Jardin\Llamadores.html</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>246</v>
+      <c r="C6" s="17" t="s">
+        <v>242</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="E6" s="7">
         <v>1</v>
@@ -1648,19 +1748,36 @@
       <c r="G6" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="30"/>
+      <c r="I6" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Jardin/Veletas.html</v>
+      </c>
+      <c r="J6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Jardin/Veletas</v>
+      </c>
+      <c r="K6" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Jardin\Veletas</v>
+      </c>
+      <c r="L6" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Jardin\Veletas.html</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>247</v>
+      <c r="C7" s="17" t="s">
+        <v>243</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="E7" s="7">
         <v>1</v>
@@ -1671,19 +1788,36 @@
       <c r="G7" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="30"/>
+      <c r="I7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Jardin/Muebles-de-Jardin.html</v>
+      </c>
+      <c r="J7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Jardin/Muebles-de-Jardin</v>
+      </c>
+      <c r="K7" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Jardin\Muebles-de-Jardin</v>
+      </c>
+      <c r="L7" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Jardin\Muebles-de-Jardin.html</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>274</v>
+        <v>266</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>268</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="E8" s="7">
         <v>6</v>
@@ -1694,19 +1828,36 @@
       <c r="G8" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="30"/>
+      <c r="I8" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Jardin/Muebles-de-Jardin/Muebles-de-jardin-en-fundicion-de-aluminio.html</v>
+      </c>
+      <c r="J8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Jardin/Muebles-de-Jardin/Muebles-de-jardin-en-fundicion-de-aluminio</v>
+      </c>
+      <c r="K8" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Jardin\Muebles-de-Jardin\Muebles-de-jardin-en-fundicion-de-aluminio</v>
+      </c>
+      <c r="L8" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Jardin\Muebles-de-Jardin\Muebles-de-jardin-en-fundicion-de-aluminio.html</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>275</v>
+        <v>267</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>269</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="E9" s="7">
         <v>6</v>
@@ -1717,19 +1868,36 @@
       <c r="G9" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="30"/>
+      <c r="I9" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Jardin/Muebles-de-Jardin/Muebles-de-jardin-en-fundicion-de-hierro.html</v>
+      </c>
+      <c r="J9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Jardin/Muebles-de-Jardin/Muebles-de-jardin-en-fundicion-de-hierro</v>
+      </c>
+      <c r="K9" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Jardin\Muebles-de-Jardin\Muebles-de-jardin-en-fundicion-de-hierro</v>
+      </c>
+      <c r="L9" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Jardin\Muebles-de-Jardin\Muebles-de-jardin-en-fundicion-de-hierro.html</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>303</v>
+        <v>294</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>295</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="E10" s="7">
         <v>6</v>
@@ -1740,19 +1908,36 @@
       <c r="G10" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="30"/>
+      <c r="I10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Jardin/Muebles-de-Jardin/Muebles-de-jardin-en-hierro-forjado.html</v>
+      </c>
+      <c r="J10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Jardin/Muebles-de-Jardin/Muebles-de-jardin-en-hierro-forjado</v>
+      </c>
+      <c r="K10" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Jardin\Muebles-de-Jardin\Muebles-de-jardin-en-hierro-forjado</v>
+      </c>
+      <c r="L10" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Jardin\Muebles-de-Jardin\Muebles-de-jardin-en-hierro-forjado.html</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>248</v>
+      <c r="C11" s="18" t="s">
+        <v>244</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>8</v>
@@ -1760,19 +1945,36 @@
       <c r="G11" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="30"/>
+      <c r="I11" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Parrillas.html</v>
+      </c>
+      <c r="J11" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Parrillas</v>
+      </c>
+      <c r="K11" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Parrillas</v>
+      </c>
+      <c r="L11" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Parrillas.html</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>253</v>
+      <c r="C12" s="19" t="s">
+        <v>249</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E12" s="8">
         <v>10</v>
@@ -1783,19 +1985,36 @@
       <c r="G12" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="30"/>
+      <c r="I12" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Parrillas/Accesorios-para-parrillas.html</v>
+      </c>
+      <c r="J12" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Parrillas/Accesorios-para-parrillas</v>
+      </c>
+      <c r="K12" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Parrillas\Accesorios-para-parrillas</v>
+      </c>
+      <c r="L12" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Parrillas\Accesorios-para-parrillas.html</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>254</v>
+      <c r="C13" s="19" t="s">
+        <v>250</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E13" s="8">
         <v>10</v>
@@ -1806,19 +2025,36 @@
       <c r="G13" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="30"/>
+      <c r="I13" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Parrillas/Asadores.html</v>
+      </c>
+      <c r="J13" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Parrillas/Asadores</v>
+      </c>
+      <c r="K13" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Parrillas\Asadores</v>
+      </c>
+      <c r="L13" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Parrillas\Asadores.html</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>255</v>
+      <c r="C14" s="19" t="s">
+        <v>251</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E14" s="8">
         <v>10</v>
@@ -1829,19 +2065,36 @@
       <c r="G14" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="30"/>
+      <c r="I14" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Parrillas/Herrajes.html</v>
+      </c>
+      <c r="J14" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Parrillas/Herrajes</v>
+      </c>
+      <c r="K14" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Parrillas\Herrajes</v>
+      </c>
+      <c r="L14" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Parrillas\Herrajes.html</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>276</v>
+      <c r="C15" s="19" t="s">
+        <v>270</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E15" s="8">
         <v>10</v>
@@ -1852,19 +2105,36 @@
       <c r="G15" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="30"/>
+      <c r="I15" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Parrillas/Parrillas-a-carbon-o-lena.html</v>
+      </c>
+      <c r="J15" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Parrillas/Parrillas-a-carbon-o-lena</v>
+      </c>
+      <c r="K15" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Parrillas\Parrillas-a-carbon-o-lena</v>
+      </c>
+      <c r="L15" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Parrillas\Parrillas-a-carbon-o-lena.html</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>256</v>
+      <c r="C16" s="19" t="s">
+        <v>252</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E16" s="8">
         <v>10</v>
@@ -1875,19 +2145,36 @@
       <c r="G16" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="30"/>
+      <c r="I16" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Parrillas/Parrillas-a-gas.html</v>
+      </c>
+      <c r="J16" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Parrillas/Parrillas-a-gas</v>
+      </c>
+      <c r="K16" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Parrillas\Parrillas-a-gas</v>
+      </c>
+      <c r="L16" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Parrillas\Parrillas-a-gas.html</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>249</v>
+      <c r="C17" s="20" t="s">
+        <v>245</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>8</v>
@@ -1895,19 +2182,36 @@
       <c r="G17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="30"/>
+      <c r="I17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Calefaccion.html</v>
+      </c>
+      <c r="J17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Calefaccion</v>
+      </c>
+      <c r="K17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Calefaccion</v>
+      </c>
+      <c r="L17" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Calefaccion.html</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>257</v>
+      <c r="C18" s="21" t="s">
+        <v>253</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="E18" s="2">
         <v>16</v>
@@ -1918,19 +2222,36 @@
       <c r="G18" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="30"/>
+      <c r="I18" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Calefaccion/Hogares.html</v>
+      </c>
+      <c r="J18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Calefaccion/Hogares</v>
+      </c>
+      <c r="K18" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Calefaccion\Hogares</v>
+      </c>
+      <c r="L18" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Calefaccion\Hogares.html</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>18</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>250</v>
+      <c r="C19" s="22" t="s">
+        <v>246</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>8</v>
@@ -1938,19 +2259,36 @@
       <c r="G19" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="30"/>
+      <c r="I19" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Iluminacion.html</v>
+      </c>
+      <c r="J19" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Iluminacion</v>
+      </c>
+      <c r="K19" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Iluminacion</v>
+      </c>
+      <c r="L19" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Iluminacion.html</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>258</v>
+      <c r="C20" s="23" t="s">
+        <v>254</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E20" s="10">
         <v>18</v>
@@ -1961,19 +2299,36 @@
       <c r="G20" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="30"/>
+      <c r="I20" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Iluminacion/Faroles.html</v>
+      </c>
+      <c r="J20" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Iluminacion/Faroles</v>
+      </c>
+      <c r="K20" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Iluminacion\Faroles</v>
+      </c>
+      <c r="L20" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Iluminacion\Faroles.html</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>259</v>
+      <c r="C21" s="23" t="s">
+        <v>255</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="E21" s="10">
         <v>18</v>
@@ -1984,19 +2339,36 @@
       <c r="G21" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="30"/>
+      <c r="I21" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Iluminacion/Faroles-con-columnas.html</v>
+      </c>
+      <c r="J21" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Iluminacion/Faroles-con-columnas</v>
+      </c>
+      <c r="K21" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Iluminacion\Faroles-con-columnas</v>
+      </c>
+      <c r="L21" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Iluminacion\Faroles-con-columnas.html</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>21</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>251</v>
+      <c r="C22" s="24" t="s">
+        <v>247</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>8</v>
@@ -2004,16 +2376,33 @@
       <c r="G22" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="30"/>
+      <c r="I22" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia.html</v>
+      </c>
+      <c r="J22" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Gastronomia</v>
+      </c>
+      <c r="K22" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia</v>
+      </c>
+      <c r="L22" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia.html</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>22</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>260</v>
+      <c r="C23" s="25" t="s">
+        <v>256</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>180</v>
@@ -2027,16 +2416,33 @@
       <c r="G23" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="30"/>
+      <c r="I23" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Calderos-en-hierro.html</v>
+      </c>
+      <c r="J23" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Gastronomia/Calderos-en-hierro</v>
+      </c>
+      <c r="K23" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Calderos-en-hierro</v>
+      </c>
+      <c r="L23" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Calderos-en-hierro.html</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>261</v>
+      <c r="C24" s="25" t="s">
+        <v>257</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>183</v>
@@ -2050,19 +2456,36 @@
       <c r="G24" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="30"/>
+      <c r="I24" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Cacerolas-de-fundicion.html</v>
+      </c>
+      <c r="J24" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Gastronomia/Cacerolas-de-fundicion</v>
+      </c>
+      <c r="K24" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Cacerolas-de-fundicion</v>
+      </c>
+      <c r="L24" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Cacerolas-de-fundicion.html</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>306</v>
+        <v>297</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>298</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="E25" s="3">
         <v>23</v>
@@ -2073,19 +2496,36 @@
       <c r="G25" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="30"/>
+      <c r="I25" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Cacerolas-de-fundicion/Cacerolas-de-fundicion-enlozadas.html</v>
+      </c>
+      <c r="J25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Gastronomia/Cacerolas-de-fundicion/Cacerolas-de-fundicion-enlozadas</v>
+      </c>
+      <c r="K25" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Cacerolas-de-fundicion\Cacerolas-de-fundicion-enlozadas</v>
+      </c>
+      <c r="L25" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Cacerolas-de-fundicion\Cacerolas-de-fundicion-enlozadas.html</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>309</v>
+        <v>300</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>301</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="E26" s="3">
         <v>23</v>
@@ -2096,19 +2536,36 @@
       <c r="G26" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="30"/>
+      <c r="I26" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Cacerolas-de-fundicion/Cacerolas-de-fundicion-sin-enlozar.html</v>
+      </c>
+      <c r="J26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Gastronomia/Cacerolas-de-fundicion/Cacerolas-de-fundicion-sin-enlozar</v>
+      </c>
+      <c r="K26" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Cacerolas-de-fundicion\Cacerolas-de-fundicion-sin-enlozar</v>
+      </c>
+      <c r="L26" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Cacerolas-de-fundicion\Cacerolas-de-fundicion-sin-enlozar.html</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>26</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>311</v>
+        <v>346</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>326</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="E27" s="13">
         <v>25</v>
@@ -2119,19 +2576,36 @@
       <c r="G27" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H27" s="30"/>
+      <c r="I27" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Cacerolas-de-fundicion/Cacerolas-de-fundicion-sin-enlozar/Cacerolas-de-fundicion-sin-enlozar-ovaladas.html</v>
+      </c>
+      <c r="J27" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Gastronomia/Cacerolas-de-fundicion/Cacerolas-de-fundicion-sin-enlozar/Cacerolas-de-fundicion-sin-enlozar-ovaladas</v>
+      </c>
+      <c r="K27" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Cacerolas-de-fundicion\Cacerolas-de-fundicion-sin-enlozar\Cacerolas-de-fundicion-sin-enlozar-ovaladas</v>
+      </c>
+      <c r="L27" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Cacerolas-de-fundicion\Cacerolas-de-fundicion-sin-enlozar\Cacerolas-de-fundicion-sin-enlozar-ovaladas.html</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>27</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>312</v>
+        <v>347</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>327</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E28" s="13">
         <v>25</v>
@@ -2142,16 +2616,33 @@
       <c r="G28" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="30"/>
+      <c r="I28" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Cacerolas-de-fundicion/Cacerolas-de-fundicion-sin-enlozar/Cacerolas-de-fundicion-sin-enlozar-doble-funcion.html</v>
+      </c>
+      <c r="J28" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Gastronomia/Cacerolas-de-fundicion/Cacerolas-de-fundicion-sin-enlozar/Cacerolas-de-fundicion-sin-enlozar-doble-funcion</v>
+      </c>
+      <c r="K28" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Cacerolas-de-fundicion\Cacerolas-de-fundicion-sin-enlozar\Cacerolas-de-fundicion-sin-enlozar-doble-funcion</v>
+      </c>
+      <c r="L28" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Cacerolas-de-fundicion\Cacerolas-de-fundicion-sin-enlozar\Cacerolas-de-fundicion-sin-enlozar-doble-funcion.html</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>262</v>
+      <c r="C29" s="25" t="s">
+        <v>258</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>193</v>
@@ -2165,16 +2656,33 @@
       <c r="G29" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="30"/>
+      <c r="I29" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Planchas-para-bifes.html</v>
+      </c>
+      <c r="J29" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Gastronomia/Planchas-para-bifes</v>
+      </c>
+      <c r="K29" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Planchas-para-bifes</v>
+      </c>
+      <c r="L29" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Planchas-para-bifes.html</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>29</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>268</v>
+        <v>236</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>264</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>195</v>
@@ -2188,16 +2696,33 @@
       <c r="G30" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="30"/>
+      <c r="I30" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Planchas-para-bifes/Planchas-para-bifes-lisas.html</v>
+      </c>
+      <c r="J30" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Gastronomia/Planchas-para-bifes/Planchas-para-bifes-lisas</v>
+      </c>
+      <c r="K30" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Planchas-para-bifes\Planchas-para-bifes-lisas</v>
+      </c>
+      <c r="L30" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Planchas-para-bifes\Planchas-para-bifes-lisas.html</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>269</v>
+        <v>237</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>265</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>197</v>
@@ -2211,16 +2736,33 @@
       <c r="G31" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="30"/>
+      <c r="I31" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Planchas-para-bifes/Planchas-para-bifes-rayadas.html</v>
+      </c>
+      <c r="J31" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Gastronomia/Planchas-para-bifes/Planchas-para-bifes-rayadas</v>
+      </c>
+      <c r="K31" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Planchas-para-bifes\Planchas-para-bifes-rayadas</v>
+      </c>
+      <c r="L31" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Planchas-para-bifes\Planchas-para-bifes-rayadas.html</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>314</v>
+        <v>303</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>304</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>199</v>
@@ -2234,16 +2776,33 @@
       <c r="G32" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H32" s="30"/>
+      <c r="I32" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Planchas-para-bifes/Planchas-para-bifes-rayadas/Planchas-para-bifes-rayadas-enlozadas.html</v>
+      </c>
+      <c r="J32" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Gastronomia/Planchas-para-bifes/Planchas-para-bifes-rayadas/Planchas-para-bifes-rayadas-enlozadas</v>
+      </c>
+      <c r="K32" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Planchas-para-bifes\Planchas-para-bifes-rayadas\Planchas-para-bifes-rayadas-enlozadas</v>
+      </c>
+      <c r="L32" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Planchas-para-bifes\Planchas-para-bifes-rayadas\Planchas-para-bifes-rayadas-enlozadas.html</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>316</v>
+        <v>305</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>306</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>201</v>
@@ -2257,19 +2816,36 @@
       <c r="G33" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="30"/>
+      <c r="I33" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Planchas-para-bifes/Planchas-para-bifes-rayadas/Planchas-para-bifes-rayadas-sin-enlozar.html</v>
+      </c>
+      <c r="J33" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Categorias/Gastronomia/Planchas-para-bifes/Planchas-para-bifes-rayadas/Planchas-para-bifes-rayadas-sin-enlozar</v>
+      </c>
+      <c r="K33" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Planchas-para-bifes\Planchas-para-bifes-rayadas\Planchas-para-bifes-rayadas-sin-enlozar</v>
+      </c>
+      <c r="L33" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Planchas-para-bifes\Planchas-para-bifes-rayadas\Planchas-para-bifes-rayadas-sin-enlozar.html</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>33</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="12" t="s">
-        <v>263</v>
+      <c r="C34" s="25" t="s">
+        <v>259</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="E34" s="12">
         <v>21</v>
@@ -2280,19 +2856,36 @@
       <c r="G34" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="30"/>
+      <c r="I34" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion.html</v>
+      </c>
+      <c r="J34" s="12" t="str">
+        <f t="shared" ref="J34:J52" si="4">SUBSTITUTE(I34,".html","")</f>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion</v>
+      </c>
+      <c r="K34" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Provoleteras-de-fundicion</v>
+      </c>
+      <c r="L34" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Provoleteras-de-fundicion.html</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>240</v>
-      </c>
-      <c r="C35" t="s">
-        <v>270</v>
+        <v>332</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>328</v>
       </c>
       <c r="D35" t="s">
-        <v>299</v>
+        <v>333</v>
       </c>
       <c r="E35">
         <v>33</v>
@@ -2303,19 +2896,35 @@
       <c r="G35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-madera.html</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-madera</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-fundicion-mango-de-madera</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-fundicion-mango-de-madera.html</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>317</v>
-      </c>
-      <c r="C36" t="s">
-        <v>318</v>
+        <v>334</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>329</v>
       </c>
       <c r="D36" t="s">
-        <v>319</v>
+        <v>335</v>
       </c>
       <c r="E36">
         <v>34</v>
@@ -2326,19 +2935,35 @@
       <c r="G36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-madera/Provoleteras-de-fundicion-mango-de-madera-enlozadas.html</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-madera/Provoleteras-de-fundicion-mango-de-madera-enlozadas</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-fundicion-mango-de-madera\Provoleteras-de-fundicion-mango-de-madera-enlozadas</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-fundicion-mango-de-madera\Provoleteras-de-fundicion-mango-de-madera-enlozadas.html</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>320</v>
-      </c>
-      <c r="C37" t="s">
-        <v>321</v>
+        <v>336</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>330</v>
       </c>
       <c r="D37" t="s">
-        <v>322</v>
+        <v>337</v>
       </c>
       <c r="E37">
         <v>34</v>
@@ -2349,19 +2974,35 @@
       <c r="G37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I37" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-madera/Provoleteras-de-fundicion-mango-de-madera-sin-enlozar.html</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-madera/Provoleteras-de-fundicion-mango-de-madera-sin-enlozar</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-fundicion-mango-de-madera\Provoleteras-de-fundicion-mango-de-madera-sin-enlozar</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-fundicion-mango-de-madera\Provoleteras-de-fundicion-mango-de-madera-sin-enlozar.html</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>241</v>
-      </c>
-      <c r="C38" t="s">
-        <v>271</v>
+        <v>338</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>331</v>
       </c>
       <c r="D38" t="s">
-        <v>300</v>
+        <v>339</v>
       </c>
       <c r="E38">
         <v>33</v>
@@ -2372,19 +3013,35 @@
       <c r="G38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I38" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion.html</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-fundicion-mango-de-fundicion</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-fundicion-mango-de-fundicion.html</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>346</v>
-      </c>
-      <c r="C39" t="s">
-        <v>323</v>
+        <v>340</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>341</v>
       </c>
       <c r="D39" t="s">
-        <v>324</v>
+        <v>342</v>
       </c>
       <c r="E39">
         <v>37</v>
@@ -2395,19 +3052,35 @@
       <c r="G39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I39" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion-enlozadas.html</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion-enlozadas</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-fundicion-mango-de-fundicion\Provoleteras-de-fundicion-mango-de-fundicion-enlozadas</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-fundicion-mango-de-fundicion\Provoleteras-de-fundicion-mango-de-fundicion-enlozadas.html</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>348</v>
-      </c>
-      <c r="C40" t="s">
-        <v>325</v>
+        <v>343</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>344</v>
       </c>
       <c r="D40" t="s">
-        <v>326</v>
+        <v>345</v>
       </c>
       <c r="E40">
         <v>37</v>
@@ -2418,19 +3091,35 @@
       <c r="G40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I40" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion-sin-enlozar.html</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion-sin-enlozar</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-fundicion-mango-de-fundicion\Provoleteras-de-fundicion-mango-de-fundicion-sin-enlozar</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-fundicion-mango-de-fundicion\Provoleteras-de-fundicion-mango-de-fundicion-sin-enlozar.html</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>242</v>
-      </c>
-      <c r="C41" t="s">
-        <v>277</v>
+        <v>238</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>271</v>
       </c>
       <c r="D41" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="E41">
         <v>33</v>
@@ -2441,19 +3130,35 @@
       <c r="G41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I41" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-15-porciones.html</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-15-porciones</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-15-porciones</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-15-porciones.html</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>327</v>
-      </c>
-      <c r="C42" t="s">
-        <v>328</v>
+        <v>307</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>308</v>
       </c>
       <c r="D42" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="E42">
         <v>40</v>
@@ -2464,19 +3169,35 @@
       <c r="G42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I42" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-15-porciones/Provoleteras-de-15-porciones-enlozadas.html</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-15-porciones/Provoleteras-de-15-porciones-enlozadas</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-15-porciones\Provoleteras-de-15-porciones-enlozadas</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-15-porciones\Provoleteras-de-15-porciones-enlozadas.html</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>330</v>
-      </c>
-      <c r="C43" t="s">
-        <v>331</v>
+        <v>310</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>311</v>
       </c>
       <c r="D43" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="E43">
         <v>40</v>
@@ -2487,16 +3208,32 @@
       <c r="G43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I43" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-15-porciones/Provoleteras-de-15-porciones-sin-enlozar.html</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-15-porciones/Provoleteras-de-15-porciones-sin-enlozar</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-15-porciones\Provoleteras-de-15-porciones-sin-enlozar</v>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Provoleteras-de-fundicion\Provoleteras-de-15-porciones\Provoleteras-de-15-porciones-sin-enlozar.html</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <v>43</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="C44" s="12" t="s">
-        <v>264</v>
+      <c r="C44" s="25" t="s">
+        <v>260</v>
       </c>
       <c r="D44" s="12" t="s">
         <v>219</v>
@@ -2510,8 +3247,25 @@
       <c r="G44" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="30"/>
+      <c r="I44" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Asaderas-en-chapa-plegada.html</v>
+      </c>
+      <c r="J44" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Asaderas-en-chapa-plegada</v>
+      </c>
+      <c r="K44" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Asaderas-en-chapa-plegada</v>
+      </c>
+      <c r="L44" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Asaderas-en-chapa-plegada.html</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <v>44</v>
       </c>
@@ -2519,7 +3273,7 @@
         <v>119</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>221</v>
@@ -2533,19 +3287,36 @@
       <c r="G45" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="30"/>
+      <c r="I45" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Paelleras-con-2-asas.html</v>
+      </c>
+      <c r="J45" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Paelleras-con-2-asas</v>
+      </c>
+      <c r="K45" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Paelleras-con-2-asas</v>
+      </c>
+      <c r="L45" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Paelleras-con-2-asas.html</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>333</v>
-      </c>
-      <c r="C46" t="s">
-        <v>334</v>
+        <v>313</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>314</v>
       </c>
       <c r="D46" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="E46">
         <v>44</v>
@@ -2556,19 +3327,35 @@
       <c r="G46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I46" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Paelleras-con-2-asas/Paelleras-con-2-asas-enlozadas.html</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Paelleras-con-2-asas/Paelleras-con-2-asas-enlozadas</v>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Paelleras-con-2-asas\Paelleras-con-2-asas-enlozadas</v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Paelleras-con-2-asas\Paelleras-con-2-asas-enlozadas.html</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>336</v>
-      </c>
-      <c r="C47" t="s">
-        <v>337</v>
+        <v>316</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>317</v>
       </c>
       <c r="D47" t="s">
-        <v>338</v>
+        <v>318</v>
       </c>
       <c r="E47">
         <v>44</v>
@@ -2579,16 +3366,32 @@
       <c r="G47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I47" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Paelleras-con-2-asas/Paelleras-con-2-asas-sin-enlozar.html</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Paelleras-con-2-asas/Paelleras-con-2-asas-sin-enlozar</v>
+      </c>
+      <c r="K47" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Paelleras-con-2-asas\Paelleras-con-2-asas-sin-enlozar</v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Paelleras-con-2-asas\Paelleras-con-2-asas-sin-enlozar.html</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>47</v>
       </c>
       <c r="B48" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C48" s="12" t="s">
-        <v>266</v>
+      <c r="C48" s="25" t="s">
+        <v>262</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>227</v>
@@ -2602,19 +3405,36 @@
       <c r="G48" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="30"/>
+      <c r="I48" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Woks.html</v>
+      </c>
+      <c r="J48" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Woks</v>
+      </c>
+      <c r="K48" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Woks</v>
+      </c>
+      <c r="L48" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Woks.html</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>339</v>
-      </c>
-      <c r="C49" t="s">
-        <v>340</v>
+        <v>319</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>320</v>
       </c>
       <c r="D49" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
       <c r="E49">
         <v>47</v>
@@ -2625,19 +3445,35 @@
       <c r="G49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I49" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Woks/Woks-enlozados.html</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Woks/Woks-enlozados</v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Woks\Woks-enlozados</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Woks\Woks-enlozados.html</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>342</v>
-      </c>
-      <c r="C50" t="s">
-        <v>343</v>
+        <v>322</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>323</v>
       </c>
       <c r="D50" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
       <c r="E50">
         <v>47</v>
@@ -2648,8 +3484,24 @@
       <c r="G50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I50" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Woks/Woks-sin-enlozar.html</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Woks/Woks-sin-enlozar</v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Woks\Woks-sin-enlozar</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Woks\Woks-sin-enlozar.html</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
         <v>50</v>
       </c>
@@ -2657,7 +3509,7 @@
         <v>140</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="D51" s="12" t="s">
         <v>233</v>
@@ -2671,8 +3523,25 @@
       <c r="G51" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H51" s="30"/>
+      <c r="I51" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Sarten-mango-de-planchuela.html</v>
+      </c>
+      <c r="J51" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Sarten-mango-de-planchuela</v>
+      </c>
+      <c r="K51" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Sarten-mango-de-planchuela</v>
+      </c>
+      <c r="L51" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Sarten-mango-de-planchuela.html</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
         <v>51</v>
       </c>
@@ -2680,7 +3549,7 @@
         <v>144</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>235</v>
@@ -2694,15 +3563,22 @@
       <c r="G52" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
-        <v>347</v>
+      <c r="H52" s="30"/>
+      <c r="I52" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Categorias/Gastronomia/Pizzera-en-chapa-enlozada.html</v>
+      </c>
+      <c r="J52" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>Categorias/Gastronomia/Pizzera-en-chapa-enlozada</v>
+      </c>
+      <c r="K52" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>Categorias\Gastronomia\Pizzera-en-chapa-enlozada</v>
+      </c>
+      <c r="L52" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>copy plantilla-categorias.html Categorias\Gastronomia\Pizzera-en-chapa-enlozada.html</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglo de error en productos de la misma categoria
</commit_message>
<xml_diff>
--- a/productos/categorias.xlsx
+++ b/productos/categorias.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="361">
   <si>
     <t>Rayadas</t>
   </si>
@@ -1079,6 +1079,39 @@
   </si>
   <si>
     <t>Para usar el COPY para copiar la plantilla a todas las carpetas</t>
+  </si>
+  <si>
+    <t>Fundición de hierro</t>
+  </si>
+  <si>
+    <t>hierro forjado</t>
+  </si>
+  <si>
+    <t>enlozadas</t>
+  </si>
+  <si>
+    <t>sin enlozar</t>
+  </si>
+  <si>
+    <t>ovaladas</t>
+  </si>
+  <si>
+    <t>doble función</t>
+  </si>
+  <si>
+    <t>lisas</t>
+  </si>
+  <si>
+    <t>rayadas</t>
+  </si>
+  <si>
+    <t>mango de madera</t>
+  </si>
+  <si>
+    <t>mango de fundición</t>
+  </si>
+  <si>
+    <t>enlozados</t>
   </si>
 </sst>
 </file>
@@ -1518,11 +1551,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2:L52"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1534,7 +1567,7 @@
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="53" style="30" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="1.140625" customWidth="1"/>
     <col min="11" max="11" width="147.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="152.140625" bestFit="1" customWidth="1"/>
@@ -1588,7 +1621,9 @@
       <c r="G2" s="6">
         <v>0</v>
       </c>
-      <c r="H2" s="30"/>
+      <c r="H2" t="s">
+        <v>148</v>
+      </c>
       <c r="I2" s="6" t="str">
         <f>SUBSTITUTE(C2,"/productos/","")</f>
         <v>Categorias/Jardin.html</v>
@@ -1628,7 +1663,9 @@
       <c r="G3" s="7">
         <v>1</v>
       </c>
-      <c r="H3" s="30"/>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
       <c r="I3" s="7" t="str">
         <f t="shared" ref="I3:I52" si="1">SUBSTITUTE(C3,"/productos/","")</f>
         <v>Categorias/Jardin/Arrollamangueras.html</v>
@@ -1668,7 +1705,9 @@
       <c r="G4" s="7">
         <v>1</v>
       </c>
-      <c r="H4" s="30"/>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
       <c r="I4" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Jardin/Bebederos.html</v>
@@ -1708,7 +1747,9 @@
       <c r="G5" s="7">
         <v>0</v>
       </c>
-      <c r="H5" s="30"/>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
       <c r="I5" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Jardin/Llamadores.html</v>
@@ -1748,7 +1789,9 @@
       <c r="G6" s="7">
         <v>0</v>
       </c>
-      <c r="H6" s="30"/>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
       <c r="I6" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Jardin/Veletas.html</v>
@@ -1788,7 +1831,9 @@
       <c r="G7" s="7">
         <v>0</v>
       </c>
-      <c r="H7" s="30"/>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
       <c r="I7" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Jardin/Muebles-de-Jardin.html</v>
@@ -1828,7 +1873,9 @@
       <c r="G8" s="7">
         <v>0</v>
       </c>
-      <c r="H8" s="30"/>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
       <c r="I8" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Jardin/Muebles-de-Jardin/Muebles-de-jardin-en-fundicion-de-aluminio.html</v>
@@ -1868,7 +1915,9 @@
       <c r="G9" s="7">
         <v>0</v>
       </c>
-      <c r="H9" s="30"/>
+      <c r="H9" t="s">
+        <v>350</v>
+      </c>
       <c r="I9" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Jardin/Muebles-de-Jardin/Muebles-de-jardin-en-fundicion-de-hierro.html</v>
@@ -1908,7 +1957,9 @@
       <c r="G10" s="7">
         <v>0</v>
       </c>
-      <c r="H10" s="30"/>
+      <c r="H10" t="s">
+        <v>351</v>
+      </c>
       <c r="I10" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Jardin/Muebles-de-Jardin/Muebles-de-jardin-en-hierro-forjado.html</v>
@@ -1945,7 +1996,9 @@
       <c r="G11" s="5">
         <v>0</v>
       </c>
-      <c r="H11" s="30"/>
+      <c r="H11" t="s">
+        <v>163</v>
+      </c>
       <c r="I11" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Parrillas.html</v>
@@ -1985,7 +2038,9 @@
       <c r="G12" s="8">
         <v>0</v>
       </c>
-      <c r="H12" s="30"/>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
       <c r="I12" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Parrillas/Accesorios-para-parrillas.html</v>
@@ -2025,7 +2080,9 @@
       <c r="G13" s="8">
         <v>0</v>
       </c>
-      <c r="H13" s="30"/>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
       <c r="I13" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Parrillas/Asadores.html</v>
@@ -2065,7 +2122,9 @@
       <c r="G14" s="8">
         <v>0</v>
       </c>
-      <c r="H14" s="30"/>
+      <c r="H14" t="s">
+        <v>25</v>
+      </c>
       <c r="I14" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Parrillas/Herrajes.html</v>
@@ -2105,7 +2164,9 @@
       <c r="G15" s="8">
         <v>0</v>
       </c>
-      <c r="H15" s="30"/>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
       <c r="I15" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Parrillas/Parrillas-a-carbon-o-lena.html</v>
@@ -2145,7 +2206,9 @@
       <c r="G16" s="8">
         <v>0</v>
       </c>
-      <c r="H16" s="30"/>
+      <c r="H16" t="s">
+        <v>29</v>
+      </c>
       <c r="I16" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Parrillas/Parrillas-a-gas.html</v>
@@ -2182,7 +2245,9 @@
       <c r="G17" s="1">
         <v>0</v>
       </c>
-      <c r="H17" s="30"/>
+      <c r="H17" t="s">
+        <v>170</v>
+      </c>
       <c r="I17" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Calefaccion.html</v>
@@ -2222,7 +2287,9 @@
       <c r="G18" s="2">
         <v>0</v>
       </c>
-      <c r="H18" s="30"/>
+      <c r="H18" t="s">
+        <v>31</v>
+      </c>
       <c r="I18" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Calefaccion/Hogares.html</v>
@@ -2259,7 +2326,9 @@
       <c r="G19" s="11">
         <v>0</v>
       </c>
-      <c r="H19" s="30"/>
+      <c r="H19" t="s">
+        <v>173</v>
+      </c>
       <c r="I19" s="11" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Iluminacion.html</v>
@@ -2299,7 +2368,9 @@
       <c r="G20" s="10">
         <v>0</v>
       </c>
-      <c r="H20" s="30"/>
+      <c r="H20" t="s">
+        <v>34</v>
+      </c>
       <c r="I20" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Iluminacion/Faroles.html</v>
@@ -2339,7 +2410,9 @@
       <c r="G21" s="10">
         <v>0</v>
       </c>
-      <c r="H21" s="30"/>
+      <c r="H21" t="s">
+        <v>36</v>
+      </c>
       <c r="I21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Iluminacion/Faroles-con-columnas.html</v>
@@ -2376,7 +2449,9 @@
       <c r="G22" s="14">
         <v>0</v>
       </c>
-      <c r="H22" s="30"/>
+      <c r="H22" t="s">
+        <v>177</v>
+      </c>
       <c r="I22" s="14" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia.html</v>
@@ -2416,7 +2491,9 @@
       <c r="G23" s="12">
         <v>0</v>
       </c>
-      <c r="H23" s="30"/>
+      <c r="H23" t="s">
+        <v>37</v>
+      </c>
       <c r="I23" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Calderos-en-hierro.html</v>
@@ -2456,7 +2533,9 @@
       <c r="G24" s="12">
         <v>0</v>
       </c>
-      <c r="H24" s="30"/>
+      <c r="H24" t="s">
+        <v>181</v>
+      </c>
       <c r="I24" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Cacerolas-de-fundicion.html</v>
@@ -2496,7 +2575,9 @@
       <c r="G25" s="3">
         <v>0</v>
       </c>
-      <c r="H25" s="30"/>
+      <c r="H25" t="s">
+        <v>352</v>
+      </c>
       <c r="I25" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Cacerolas-de-fundicion/Cacerolas-de-fundicion-enlozadas.html</v>
@@ -2536,7 +2617,9 @@
       <c r="G26" s="3">
         <v>0</v>
       </c>
-      <c r="H26" s="30"/>
+      <c r="H26" t="s">
+        <v>353</v>
+      </c>
       <c r="I26" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Cacerolas-de-fundicion/Cacerolas-de-fundicion-sin-enlozar.html</v>
@@ -2576,7 +2659,9 @@
       <c r="G27" s="13">
         <v>0</v>
       </c>
-      <c r="H27" s="30"/>
+      <c r="H27" t="s">
+        <v>354</v>
+      </c>
       <c r="I27" s="13" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Cacerolas-de-fundicion/Cacerolas-de-fundicion-sin-enlozar/Cacerolas-de-fundicion-sin-enlozar-ovaladas.html</v>
@@ -2616,7 +2701,9 @@
       <c r="G28" s="13">
         <v>0</v>
       </c>
-      <c r="H28" s="30"/>
+      <c r="H28" t="s">
+        <v>355</v>
+      </c>
       <c r="I28" s="13" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Cacerolas-de-fundicion/Cacerolas-de-fundicion-sin-enlozar/Cacerolas-de-fundicion-sin-enlozar-doble-funcion.html</v>
@@ -2656,7 +2743,9 @@
       <c r="G29" s="12">
         <v>0</v>
       </c>
-      <c r="H29" s="30"/>
+      <c r="H29" t="s">
+        <v>43</v>
+      </c>
       <c r="I29" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Planchas-para-bifes.html</v>
@@ -2696,7 +2785,9 @@
       <c r="G30" s="9">
         <v>0</v>
       </c>
-      <c r="H30" s="30"/>
+      <c r="H30" t="s">
+        <v>356</v>
+      </c>
       <c r="I30" s="9" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Planchas-para-bifes/Planchas-para-bifes-lisas.html</v>
@@ -2736,7 +2827,9 @@
       <c r="G31" s="9">
         <v>0</v>
       </c>
-      <c r="H31" s="30"/>
+      <c r="H31" t="s">
+        <v>357</v>
+      </c>
       <c r="I31" s="9" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Planchas-para-bifes/Planchas-para-bifes-rayadas.html</v>
@@ -2776,7 +2869,9 @@
       <c r="G32" s="4">
         <v>0</v>
       </c>
-      <c r="H32" s="30"/>
+      <c r="H32" t="s">
+        <v>352</v>
+      </c>
       <c r="I32" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Planchas-para-bifes/Planchas-para-bifes-rayadas/Planchas-para-bifes-rayadas-enlozadas.html</v>
@@ -2816,7 +2911,9 @@
       <c r="G33" s="4">
         <v>0</v>
       </c>
-      <c r="H33" s="30"/>
+      <c r="H33" t="s">
+        <v>353</v>
+      </c>
       <c r="I33" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Planchas-para-bifes/Planchas-para-bifes-rayadas/Planchas-para-bifes-rayadas-sin-enlozar.html</v>
@@ -2856,7 +2953,9 @@
       <c r="G34" s="12">
         <v>1</v>
       </c>
-      <c r="H34" s="30"/>
+      <c r="H34" t="s">
+        <v>54</v>
+      </c>
       <c r="I34" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Provoleteras-de-fundicion.html</v>
@@ -2896,6 +2995,9 @@
       <c r="G35">
         <v>0</v>
       </c>
+      <c r="H35" t="s">
+        <v>358</v>
+      </c>
       <c r="I35" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-madera.html</v>
@@ -2935,6 +3037,9 @@
       <c r="G36">
         <v>0</v>
       </c>
+      <c r="H36" t="s">
+        <v>352</v>
+      </c>
       <c r="I36" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-madera/Provoleteras-de-fundicion-mango-de-madera-enlozadas.html</v>
@@ -2974,6 +3079,9 @@
       <c r="G37">
         <v>0</v>
       </c>
+      <c r="H37" t="s">
+        <v>353</v>
+      </c>
       <c r="I37" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-madera/Provoleteras-de-fundicion-mango-de-madera-sin-enlozar.html</v>
@@ -3013,6 +3121,9 @@
       <c r="G38">
         <v>0</v>
       </c>
+      <c r="H38" t="s">
+        <v>359</v>
+      </c>
       <c r="I38" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion.html</v>
@@ -3052,6 +3163,9 @@
       <c r="G39">
         <v>0</v>
       </c>
+      <c r="H39" t="s">
+        <v>352</v>
+      </c>
       <c r="I39" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion-enlozadas.html</v>
@@ -3091,6 +3205,9 @@
       <c r="G40">
         <v>0</v>
       </c>
+      <c r="H40" t="s">
+        <v>353</v>
+      </c>
       <c r="I40" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion/Provoleteras-de-fundicion-mango-de-fundicion-sin-enlozar.html</v>
@@ -3130,6 +3247,9 @@
       <c r="G41">
         <v>0</v>
       </c>
+      <c r="H41" t="s">
+        <v>238</v>
+      </c>
       <c r="I41" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-15-porciones.html</v>
@@ -3169,6 +3289,9 @@
       <c r="G42">
         <v>0</v>
       </c>
+      <c r="H42" t="s">
+        <v>352</v>
+      </c>
       <c r="I42" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-15-porciones/Provoleteras-de-15-porciones-enlozadas.html</v>
@@ -3208,6 +3331,9 @@
       <c r="G43">
         <v>0</v>
       </c>
+      <c r="H43" t="s">
+        <v>353</v>
+      </c>
       <c r="I43" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Provoleteras-de-fundicion/Provoleteras-de-15-porciones/Provoleteras-de-15-porciones-sin-enlozar.html</v>
@@ -3247,7 +3373,9 @@
       <c r="G44" s="12">
         <v>0</v>
       </c>
-      <c r="H44" s="30"/>
+      <c r="H44" t="s">
+        <v>115</v>
+      </c>
       <c r="I44" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Asaderas-en-chapa-plegada.html</v>
@@ -3287,7 +3415,9 @@
       <c r="G45" s="12">
         <v>0</v>
       </c>
-      <c r="H45" s="30"/>
+      <c r="H45" t="s">
+        <v>119</v>
+      </c>
       <c r="I45" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Paelleras-con-2-asas.html</v>
@@ -3327,6 +3457,9 @@
       <c r="G46">
         <v>0</v>
       </c>
+      <c r="H46" t="s">
+        <v>352</v>
+      </c>
       <c r="I46" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Paelleras-con-2-asas/Paelleras-con-2-asas-enlozadas.html</v>
@@ -3366,6 +3499,9 @@
       <c r="G47">
         <v>0</v>
       </c>
+      <c r="H47" t="s">
+        <v>353</v>
+      </c>
       <c r="I47" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Paelleras-con-2-asas/Paelleras-con-2-asas-sin-enlozar.html</v>
@@ -3405,7 +3541,9 @@
       <c r="G48" s="12">
         <v>0</v>
       </c>
-      <c r="H48" s="30"/>
+      <c r="H48" t="s">
+        <v>129</v>
+      </c>
       <c r="I48" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Woks.html</v>
@@ -3445,6 +3583,9 @@
       <c r="G49">
         <v>0</v>
       </c>
+      <c r="H49" t="s">
+        <v>360</v>
+      </c>
       <c r="I49" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Woks/Woks-enlozados.html</v>
@@ -3484,6 +3625,9 @@
       <c r="G50">
         <v>0</v>
       </c>
+      <c r="H50" t="s">
+        <v>353</v>
+      </c>
       <c r="I50" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Woks/Woks-sin-enlozar.html</v>
@@ -3523,7 +3667,9 @@
       <c r="G51" s="12">
         <v>0</v>
       </c>
-      <c r="H51" s="30"/>
+      <c r="H51" t="s">
+        <v>140</v>
+      </c>
       <c r="I51" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Sarten-mango-de-planchuela.html</v>
@@ -3563,7 +3709,9 @@
       <c r="G52" s="12">
         <v>0</v>
       </c>
-      <c r="H52" s="30"/>
+      <c r="H52" t="s">
+        <v>144</v>
+      </c>
       <c r="I52" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Categorias/Gastronomia/Pizzera-en-chapa-enlozada.html</v>
@@ -3579,6 +3727,1164 @@
       <c r="L52" s="12" t="str">
         <f t="shared" si="3"/>
         <v>copy plantilla-categorias.html Categorias\Gastronomia\Pizzera-en-chapa-enlozada.html</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>1</v>
+      </c>
+      <c r="B76" t="s">
+        <v>148</v>
+      </c>
+      <c r="C76" t="s">
+        <v>248</v>
+      </c>
+      <c r="D76" t="s">
+        <v>150</v>
+      </c>
+      <c r="F76" t="s">
+        <v>151</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>2</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>239</v>
+      </c>
+      <c r="D77" t="s">
+        <v>272</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77" t="s">
+        <v>4</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>3</v>
+      </c>
+      <c r="B78" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" t="s">
+        <v>240</v>
+      </c>
+      <c r="D78" t="s">
+        <v>155</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78" t="s">
+        <v>8</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>4</v>
+      </c>
+      <c r="B79" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79" t="s">
+        <v>241</v>
+      </c>
+      <c r="D79" t="s">
+        <v>273</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79" t="s">
+        <v>8</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>5</v>
+      </c>
+      <c r="B80" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80" t="s">
+        <v>242</v>
+      </c>
+      <c r="D80" t="s">
+        <v>274</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80" t="s">
+        <v>8</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>6</v>
+      </c>
+      <c r="B81" t="s">
+        <v>13</v>
+      </c>
+      <c r="C81" t="s">
+        <v>243</v>
+      </c>
+      <c r="D81" t="s">
+        <v>275</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81" t="s">
+        <v>8</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>7</v>
+      </c>
+      <c r="B82" t="s">
+        <v>266</v>
+      </c>
+      <c r="C82" t="s">
+        <v>268</v>
+      </c>
+      <c r="D82" t="s">
+        <v>276</v>
+      </c>
+      <c r="E82">
+        <v>6</v>
+      </c>
+      <c r="F82" t="s">
+        <v>8</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>8</v>
+      </c>
+      <c r="B83" t="s">
+        <v>267</v>
+      </c>
+      <c r="C83" t="s">
+        <v>269</v>
+      </c>
+      <c r="D83" t="s">
+        <v>277</v>
+      </c>
+      <c r="E83">
+        <v>6</v>
+      </c>
+      <c r="F83" t="s">
+        <v>8</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>9</v>
+      </c>
+      <c r="B84" t="s">
+        <v>294</v>
+      </c>
+      <c r="C84" t="s">
+        <v>295</v>
+      </c>
+      <c r="D84" t="s">
+        <v>296</v>
+      </c>
+      <c r="E84">
+        <v>6</v>
+      </c>
+      <c r="F84" t="s">
+        <v>8</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>10</v>
+      </c>
+      <c r="B85" t="s">
+        <v>163</v>
+      </c>
+      <c r="C85" t="s">
+        <v>244</v>
+      </c>
+      <c r="D85" t="s">
+        <v>278</v>
+      </c>
+      <c r="F85" t="s">
+        <v>8</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>11</v>
+      </c>
+      <c r="B86" t="s">
+        <v>21</v>
+      </c>
+      <c r="C86" t="s">
+        <v>249</v>
+      </c>
+      <c r="D86" t="s">
+        <v>279</v>
+      </c>
+      <c r="E86">
+        <v>10</v>
+      </c>
+      <c r="F86" t="s">
+        <v>8</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>12</v>
+      </c>
+      <c r="B87" t="s">
+        <v>23</v>
+      </c>
+      <c r="C87" t="s">
+        <v>250</v>
+      </c>
+      <c r="D87" t="s">
+        <v>280</v>
+      </c>
+      <c r="E87">
+        <v>10</v>
+      </c>
+      <c r="F87" t="s">
+        <v>8</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>13</v>
+      </c>
+      <c r="B88" t="s">
+        <v>25</v>
+      </c>
+      <c r="C88" t="s">
+        <v>251</v>
+      </c>
+      <c r="D88" t="s">
+        <v>281</v>
+      </c>
+      <c r="E88">
+        <v>10</v>
+      </c>
+      <c r="F88" t="s">
+        <v>8</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>14</v>
+      </c>
+      <c r="B89" t="s">
+        <v>27</v>
+      </c>
+      <c r="C89" t="s">
+        <v>270</v>
+      </c>
+      <c r="D89" t="s">
+        <v>282</v>
+      </c>
+      <c r="E89">
+        <v>10</v>
+      </c>
+      <c r="F89" t="s">
+        <v>8</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>15</v>
+      </c>
+      <c r="B90" t="s">
+        <v>29</v>
+      </c>
+      <c r="C90" t="s">
+        <v>252</v>
+      </c>
+      <c r="D90" t="s">
+        <v>283</v>
+      </c>
+      <c r="E90">
+        <v>10</v>
+      </c>
+      <c r="F90" t="s">
+        <v>8</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>16</v>
+      </c>
+      <c r="B91" t="s">
+        <v>170</v>
+      </c>
+      <c r="C91" t="s">
+        <v>245</v>
+      </c>
+      <c r="D91" t="s">
+        <v>284</v>
+      </c>
+      <c r="F91" t="s">
+        <v>8</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>17</v>
+      </c>
+      <c r="B92" t="s">
+        <v>31</v>
+      </c>
+      <c r="C92" t="s">
+        <v>253</v>
+      </c>
+      <c r="D92" t="s">
+        <v>285</v>
+      </c>
+      <c r="E92">
+        <v>16</v>
+      </c>
+      <c r="F92" t="s">
+        <v>33</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>18</v>
+      </c>
+      <c r="B93" t="s">
+        <v>173</v>
+      </c>
+      <c r="C93" t="s">
+        <v>246</v>
+      </c>
+      <c r="D93" t="s">
+        <v>286</v>
+      </c>
+      <c r="F93" t="s">
+        <v>8</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>19</v>
+      </c>
+      <c r="B94" t="s">
+        <v>34</v>
+      </c>
+      <c r="C94" t="s">
+        <v>254</v>
+      </c>
+      <c r="D94" t="s">
+        <v>287</v>
+      </c>
+      <c r="E94">
+        <v>18</v>
+      </c>
+      <c r="F94" t="s">
+        <v>33</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>20</v>
+      </c>
+      <c r="B95" t="s">
+        <v>36</v>
+      </c>
+      <c r="C95" t="s">
+        <v>255</v>
+      </c>
+      <c r="D95" t="s">
+        <v>288</v>
+      </c>
+      <c r="E95">
+        <v>18</v>
+      </c>
+      <c r="F95" t="s">
+        <v>33</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>21</v>
+      </c>
+      <c r="B96" t="s">
+        <v>177</v>
+      </c>
+      <c r="C96" t="s">
+        <v>247</v>
+      </c>
+      <c r="D96" t="s">
+        <v>289</v>
+      </c>
+      <c r="F96" t="s">
+        <v>8</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>22</v>
+      </c>
+      <c r="B97" t="s">
+        <v>37</v>
+      </c>
+      <c r="C97" t="s">
+        <v>256</v>
+      </c>
+      <c r="D97" t="s">
+        <v>180</v>
+      </c>
+      <c r="E97">
+        <v>21</v>
+      </c>
+      <c r="F97" t="s">
+        <v>64</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>23</v>
+      </c>
+      <c r="B98" t="s">
+        <v>181</v>
+      </c>
+      <c r="C98" t="s">
+        <v>257</v>
+      </c>
+      <c r="D98" t="s">
+        <v>183</v>
+      </c>
+      <c r="E98">
+        <v>21</v>
+      </c>
+      <c r="F98" t="s">
+        <v>67</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>24</v>
+      </c>
+      <c r="B99" t="s">
+        <v>297</v>
+      </c>
+      <c r="C99" t="s">
+        <v>298</v>
+      </c>
+      <c r="D99" t="s">
+        <v>299</v>
+      </c>
+      <c r="E99">
+        <v>23</v>
+      </c>
+      <c r="F99" t="s">
+        <v>70</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>25</v>
+      </c>
+      <c r="B100" t="s">
+        <v>300</v>
+      </c>
+      <c r="C100" t="s">
+        <v>301</v>
+      </c>
+      <c r="D100" t="s">
+        <v>302</v>
+      </c>
+      <c r="E100">
+        <v>23</v>
+      </c>
+      <c r="F100" t="s">
+        <v>73</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>26</v>
+      </c>
+      <c r="B101" t="s">
+        <v>346</v>
+      </c>
+      <c r="C101" t="s">
+        <v>326</v>
+      </c>
+      <c r="D101" t="s">
+        <v>290</v>
+      </c>
+      <c r="E101">
+        <v>25</v>
+      </c>
+      <c r="F101" t="s">
+        <v>76</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>27</v>
+      </c>
+      <c r="B102" t="s">
+        <v>347</v>
+      </c>
+      <c r="C102" t="s">
+        <v>327</v>
+      </c>
+      <c r="D102" t="s">
+        <v>291</v>
+      </c>
+      <c r="E102">
+        <v>25</v>
+      </c>
+      <c r="F102" t="s">
+        <v>79</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>28</v>
+      </c>
+      <c r="B103" t="s">
+        <v>43</v>
+      </c>
+      <c r="C103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D103" t="s">
+        <v>193</v>
+      </c>
+      <c r="E103">
+        <v>21</v>
+      </c>
+      <c r="F103" t="s">
+        <v>46</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>29</v>
+      </c>
+      <c r="B104" t="s">
+        <v>236</v>
+      </c>
+      <c r="C104" t="s">
+        <v>264</v>
+      </c>
+      <c r="D104" t="s">
+        <v>195</v>
+      </c>
+      <c r="E104">
+        <v>28</v>
+      </c>
+      <c r="F104" t="s">
+        <v>82</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>30</v>
+      </c>
+      <c r="B105" t="s">
+        <v>237</v>
+      </c>
+      <c r="C105" t="s">
+        <v>265</v>
+      </c>
+      <c r="D105" t="s">
+        <v>197</v>
+      </c>
+      <c r="E105">
+        <v>28</v>
+      </c>
+      <c r="F105" t="s">
+        <v>85</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>31</v>
+      </c>
+      <c r="B106" t="s">
+        <v>303</v>
+      </c>
+      <c r="C106" t="s">
+        <v>304</v>
+      </c>
+      <c r="D106" t="s">
+        <v>199</v>
+      </c>
+      <c r="E106">
+        <v>30</v>
+      </c>
+      <c r="F106" t="s">
+        <v>88</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>32</v>
+      </c>
+      <c r="B107" t="s">
+        <v>305</v>
+      </c>
+      <c r="C107" t="s">
+        <v>306</v>
+      </c>
+      <c r="D107" t="s">
+        <v>201</v>
+      </c>
+      <c r="E107">
+        <v>30</v>
+      </c>
+      <c r="F107" t="s">
+        <v>91</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>33</v>
+      </c>
+      <c r="B108" t="s">
+        <v>54</v>
+      </c>
+      <c r="C108" t="s">
+        <v>259</v>
+      </c>
+      <c r="D108" t="s">
+        <v>292</v>
+      </c>
+      <c r="E108">
+        <v>21</v>
+      </c>
+      <c r="F108" t="s">
+        <v>57</v>
+      </c>
+      <c r="G108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>34</v>
+      </c>
+      <c r="B109" t="s">
+        <v>332</v>
+      </c>
+      <c r="C109" t="s">
+        <v>328</v>
+      </c>
+      <c r="D109" t="s">
+        <v>333</v>
+      </c>
+      <c r="E109">
+        <v>33</v>
+      </c>
+      <c r="F109" t="s">
+        <v>94</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>35</v>
+      </c>
+      <c r="B110" t="s">
+        <v>334</v>
+      </c>
+      <c r="C110" t="s">
+        <v>329</v>
+      </c>
+      <c r="D110" t="s">
+        <v>335</v>
+      </c>
+      <c r="E110">
+        <v>34</v>
+      </c>
+      <c r="F110" t="s">
+        <v>97</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>36</v>
+      </c>
+      <c r="B111" t="s">
+        <v>336</v>
+      </c>
+      <c r="C111" t="s">
+        <v>330</v>
+      </c>
+      <c r="D111" t="s">
+        <v>337</v>
+      </c>
+      <c r="E111">
+        <v>34</v>
+      </c>
+      <c r="F111" t="s">
+        <v>100</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>37</v>
+      </c>
+      <c r="B112" t="s">
+        <v>338</v>
+      </c>
+      <c r="C112" t="s">
+        <v>331</v>
+      </c>
+      <c r="D112" t="s">
+        <v>339</v>
+      </c>
+      <c r="E112">
+        <v>33</v>
+      </c>
+      <c r="F112" t="s">
+        <v>103</v>
+      </c>
+      <c r="G112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>38</v>
+      </c>
+      <c r="B113" t="s">
+        <v>340</v>
+      </c>
+      <c r="C113" t="s">
+        <v>341</v>
+      </c>
+      <c r="D113" t="s">
+        <v>342</v>
+      </c>
+      <c r="E113">
+        <v>37</v>
+      </c>
+      <c r="F113" t="s">
+        <v>97</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>39</v>
+      </c>
+      <c r="B114" t="s">
+        <v>343</v>
+      </c>
+      <c r="C114" t="s">
+        <v>344</v>
+      </c>
+      <c r="D114" t="s">
+        <v>345</v>
+      </c>
+      <c r="E114">
+        <v>37</v>
+      </c>
+      <c r="F114" t="s">
+        <v>100</v>
+      </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>40</v>
+      </c>
+      <c r="B115" t="s">
+        <v>238</v>
+      </c>
+      <c r="C115" t="s">
+        <v>271</v>
+      </c>
+      <c r="D115" t="s">
+        <v>293</v>
+      </c>
+      <c r="E115">
+        <v>33</v>
+      </c>
+      <c r="F115" t="s">
+        <v>108</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>41</v>
+      </c>
+      <c r="B116" t="s">
+        <v>307</v>
+      </c>
+      <c r="C116" t="s">
+        <v>308</v>
+      </c>
+      <c r="D116" t="s">
+        <v>309</v>
+      </c>
+      <c r="E116">
+        <v>40</v>
+      </c>
+      <c r="F116" t="s">
+        <v>111</v>
+      </c>
+      <c r="G116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>42</v>
+      </c>
+      <c r="B117" t="s">
+        <v>310</v>
+      </c>
+      <c r="C117" t="s">
+        <v>311</v>
+      </c>
+      <c r="D117" t="s">
+        <v>312</v>
+      </c>
+      <c r="E117">
+        <v>40</v>
+      </c>
+      <c r="F117" t="s">
+        <v>114</v>
+      </c>
+      <c r="G117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>43</v>
+      </c>
+      <c r="B118" t="s">
+        <v>115</v>
+      </c>
+      <c r="C118" t="s">
+        <v>260</v>
+      </c>
+      <c r="D118" t="s">
+        <v>219</v>
+      </c>
+      <c r="E118">
+        <v>21</v>
+      </c>
+      <c r="F118" t="s">
+        <v>118</v>
+      </c>
+      <c r="G118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>44</v>
+      </c>
+      <c r="B119" t="s">
+        <v>119</v>
+      </c>
+      <c r="C119" t="s">
+        <v>261</v>
+      </c>
+      <c r="D119" t="s">
+        <v>221</v>
+      </c>
+      <c r="E119">
+        <v>21</v>
+      </c>
+      <c r="F119" t="s">
+        <v>122</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>45</v>
+      </c>
+      <c r="B120" t="s">
+        <v>313</v>
+      </c>
+      <c r="C120" t="s">
+        <v>314</v>
+      </c>
+      <c r="D120" t="s">
+        <v>315</v>
+      </c>
+      <c r="E120">
+        <v>44</v>
+      </c>
+      <c r="F120" t="s">
+        <v>125</v>
+      </c>
+      <c r="G120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>46</v>
+      </c>
+      <c r="B121" t="s">
+        <v>316</v>
+      </c>
+      <c r="C121" t="s">
+        <v>317</v>
+      </c>
+      <c r="D121" t="s">
+        <v>318</v>
+      </c>
+      <c r="E121">
+        <v>44</v>
+      </c>
+      <c r="F121" t="s">
+        <v>128</v>
+      </c>
+      <c r="G121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>47</v>
+      </c>
+      <c r="B122" t="s">
+        <v>129</v>
+      </c>
+      <c r="C122" t="s">
+        <v>262</v>
+      </c>
+      <c r="D122" t="s">
+        <v>227</v>
+      </c>
+      <c r="E122">
+        <v>21</v>
+      </c>
+      <c r="F122" t="s">
+        <v>132</v>
+      </c>
+      <c r="G122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>48</v>
+      </c>
+      <c r="B123" t="s">
+        <v>319</v>
+      </c>
+      <c r="C123" t="s">
+        <v>320</v>
+      </c>
+      <c r="D123" t="s">
+        <v>321</v>
+      </c>
+      <c r="E123">
+        <v>47</v>
+      </c>
+      <c r="F123" t="s">
+        <v>136</v>
+      </c>
+      <c r="G123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>49</v>
+      </c>
+      <c r="B124" t="s">
+        <v>322</v>
+      </c>
+      <c r="C124" t="s">
+        <v>323</v>
+      </c>
+      <c r="D124" t="s">
+        <v>324</v>
+      </c>
+      <c r="E124">
+        <v>47</v>
+      </c>
+      <c r="F124" t="s">
+        <v>139</v>
+      </c>
+      <c r="G124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>50</v>
+      </c>
+      <c r="B125" t="s">
+        <v>140</v>
+      </c>
+      <c r="C125" t="s">
+        <v>325</v>
+      </c>
+      <c r="D125" t="s">
+        <v>233</v>
+      </c>
+      <c r="E125">
+        <v>21</v>
+      </c>
+      <c r="F125" t="s">
+        <v>143</v>
+      </c>
+      <c r="G125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>51</v>
+      </c>
+      <c r="B126" t="s">
+        <v>144</v>
+      </c>
+      <c r="C126" t="s">
+        <v>263</v>
+      </c>
+      <c r="D126" t="s">
+        <v>235</v>
+      </c>
+      <c r="E126">
+        <v>21</v>
+      </c>
+      <c r="F126" t="s">
+        <v>147</v>
+      </c>
+      <c r="G126">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>